<commit_message>
remove empty sheet when creating new excel spreadsheet for fields
</commit_message>
<xml_diff>
--- a/ConnectStats/sqlite/out/fields.xlsx
+++ b/ConnectStats/sqlite/out/fields.xlsx
@@ -7,12 +7,11 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="gc_fields_uom" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="gc_fields_display" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="gc_fields_order" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="gc_activity_types" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="gc_category_order" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="gc_fields_uom" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="gc_fields_display" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="gc_fields_order" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="gc_activity_types" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="gc_category_order" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -350,24 +349,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:D87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2295,7 +2276,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -5547,7 +5528,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -8188,7 +8169,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -12669,7 +12650,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
Added german fields translation
</commit_message>
<xml_diff>
--- a/ConnectStats/sqlite/out/fields.xlsx
+++ b/ConnectStats/sqlite/out/fields.xlsx
@@ -3272,6 +3272,11 @@
           <t>Beginnning Latitude</t>
         </is>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Beginn Breitengrad</t>
+        </is>
+      </c>
       <c r="H2" t="inlineStr">
         <is>
           <t>開始時緯度</t>
@@ -3294,6 +3299,11 @@
           <t>Beginning Longitude</t>
         </is>
       </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Beginn Längengrad</t>
+        </is>
+      </c>
       <c r="H3" t="inlineStr">
         <is>
           <t>開始時経度</t>
@@ -3347,6 +3357,11 @@
           <t>BeginTimestamp</t>
         </is>
       </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Beginn Zeitstempel</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -3402,6 +3417,11 @@
           <t>EndLatitude</t>
         </is>
       </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Ende Breitengrad</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -3409,6 +3429,11 @@
           <t>EndLongitude</t>
         </is>
       </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Ende Längengrad</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -3452,6 +3477,11 @@
           <t>EndTimestamp</t>
         </is>
       </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Ende Zeitstempel</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -3478,7 +3508,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Positiver Höhenunterschied</t>
+          <t>Höhengewinn</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -3567,7 +3597,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Negativer Höhenunterschied</t>
+          <t>Höhenverlust</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -3680,7 +3710,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Max. Trittfrequenz (Fahrrad)</t>
+          <t>Max. Trittfrequenz (Rad)</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -3715,6 +3745,11 @@
           <t>MaxCorrectedElevation</t>
         </is>
       </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Max. korrigierte Höhe</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3734,7 +3769,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Max Run Cadence</t>
+          <t>Max. Schrittfrequenz</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -3840,7 +3875,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Max Run Cadence</t>
+          <t>Max. Schrittfrequenz</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -3906,7 +3941,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Max. HF</t>
+          <t>Max. Puls</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -3972,7 +4007,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Beste Pace</t>
+          <t>Max. Tempo</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -4012,6 +4047,11 @@
           <t>Max Power</t>
         </is>
       </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Max. Leistung</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -4024,6 +4064,11 @@
           <t>Max Avg Power (20 min)</t>
         </is>
       </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Max. Leistung 20min</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -4031,6 +4076,11 @@
           <t>MaxRelativeRunningEconomy</t>
         </is>
       </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Max. relative Laufökonomie</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -4050,7 +4100,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Max. Schrittfrequenz (Laufen)</t>
+          <t>Max. Schrittfrequenz</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -4156,7 +4206,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Maximale Schwimmfrequenz</t>
+          <t>Max. Zugfrequenz</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -4210,6 +4260,11 @@
           <t>Max Vertical Ratio</t>
         </is>
       </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Max. vertikales Verhältnis </t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -4217,6 +4272,11 @@
           <t>MaxVerticalSpeed</t>
         </is>
       </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Max. vertikale Geschw.</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -4283,6 +4343,11 @@
           <t>MinBikeCadence</t>
         </is>
       </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Min. Trittfrequenz </t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -4290,6 +4355,11 @@
           <t>MinCorrectedElevation</t>
         </is>
       </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Min. korrigierter Anstieg</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -4427,6 +4497,11 @@
           <t>Min HR</t>
         </is>
       </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Min. Puls</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -4453,6 +4528,11 @@
           <t>MinPace</t>
         </is>
       </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Min. Tempo</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -4465,6 +4545,11 @@
           <t>Min Power</t>
         </is>
       </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Min. Leistung</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -4479,6 +4564,11 @@
           <t>MinRunCadence</t>
         </is>
       </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Min. Schrittfrequenz</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -4498,7 +4588,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Min. Geschwindigkeit</t>
+          <t>Min. Geschw.</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -4545,7 +4635,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Mindestanzahl von Zügen</t>
+          <t>Min. Züge</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -4808,7 +4898,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Elapsed Time</t>
+          <t>Absolvierte Zeit</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
@@ -4890,6 +4980,11 @@
           <t>SumEnergyActive</t>
         </is>
       </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Aktivitätskalorien</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -4916,6 +5011,11 @@
           <t>Intensity Factor (IF)</t>
         </is>
       </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Intensitätsfaktor</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -5327,7 +5427,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>Training Effect</t>
+          <t>Trainingseffekt</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
@@ -5367,6 +5467,11 @@
           <t>Training Stress Score (TSS)</t>
         </is>
       </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>TSS</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -5379,6 +5484,11 @@
           <t>Threshold Power</t>
         </is>
       </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>FTP</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -5457,7 +5567,7 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>Ø Trittfrequenz (Fahrrad)</t>
+          <t>Ø Trittfrequenz (Rad)</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
@@ -5504,7 +5614,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>Avg Run Cadence</t>
+          <t>Ø Schrittfrequenz</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
@@ -5551,7 +5661,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>Durchschnittliche Effizienz</t>
+          <t>Ø Effizienz</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
@@ -5622,7 +5732,7 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>Avg Run Cadence</t>
+          <t>Ø Schrittfrequenz</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
@@ -5681,7 +5791,7 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>Avg Ground Contact Time</t>
+          <t>Ø Bodenkontaktzeit</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
@@ -5728,7 +5838,7 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>Ø HF</t>
+          <t>Ø Puls</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
@@ -5825,7 +5935,7 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>Avg Moving Pace</t>
+          <t>Ø Bewegungstempo</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
@@ -5872,7 +5982,7 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>Avg Moving Speed</t>
+          <t>Ø Bewegungsgeschw.</t>
         </is>
       </c>
       <c r="E131" t="inlineStr">
@@ -5931,7 +6041,7 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>Ø Pace</t>
+          <t>Ø Tempo</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
@@ -6009,7 +6119,7 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>Ø Schrittfrequenz (Laufen)</t>
+          <t>Ø Schrittfrequenz</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
@@ -6056,7 +6166,7 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>Ø Geschw</t>
+          <t>Ø Geschw.</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
@@ -6117,7 +6227,7 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>Avg Stride Length</t>
+          <t>Ø Zuglänge</t>
         </is>
       </c>
       <c r="E141" t="inlineStr">
@@ -6188,7 +6298,7 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>Durchschnittliche Anzahl von Zügen</t>
+          <t>Ø Anzahl von Zügen</t>
         </is>
       </c>
       <c r="E144" t="inlineStr">
@@ -6235,7 +6345,7 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>Durchschnittliche Schwimmfrequenz</t>
+          <t>Ø Zugfrequenz</t>
         </is>
       </c>
       <c r="E145" t="inlineStr">
@@ -6282,7 +6392,7 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>Durchschnittlicher SWOLF-Wert</t>
+          <t>Ø SWOLF-Wert</t>
         </is>
       </c>
       <c r="E146" t="inlineStr">
@@ -6329,7 +6439,7 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>Avg Vertical Oscillation</t>
+          <t>Ø vertikale Bewegung</t>
         </is>
       </c>
       <c r="E147" t="inlineStr">
@@ -8106,6 +8216,11 @@
           <t>SumStrokes</t>
         </is>
       </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>swimming</t>
+        </is>
+      </c>
       <c r="C92" t="inlineStr">
         <is>
           <t>dynamics</t>
@@ -8121,18 +8236,13 @@
           <t>SumStrokes</t>
         </is>
       </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>swimming</t>
-        </is>
-      </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>swim</t>
+          <t>dynamics</t>
         </is>
       </c>
       <c r="D93" t="n">
-        <v>30</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94">
@@ -9738,6 +9848,11 @@
           <t>Virtual Running</t>
         </is>
       </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Virtuelles Laufen</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -9761,6 +9876,11 @@
           <t>Obstacle Running</t>
         </is>
       </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Hindernislauf</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -9784,6 +9904,11 @@
           <t>Indoor Running</t>
         </is>
       </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Indoor-Laufen</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -10329,6 +10454,11 @@
           <t>Virtual Cycling</t>
         </is>
       </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Virtuelles Radfahren</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -11577,7 +11707,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>TENNIS</t>
+          <t>Tennis</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -11628,6 +11758,11 @@
           <t>Floor Climbing</t>
         </is>
       </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Treppensteigen</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -11651,6 +11786,11 @@
           <t>Stopwatch</t>
         </is>
       </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Stoppuhr</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -11669,6 +11809,11 @@
       <c r="D44" t="n">
         <v>4</v>
       </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Autorennen</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -11687,6 +11832,11 @@
       <c r="D45" t="n">
         <v>4</v>
       </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Atemübung</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -12401,6 +12551,11 @@
       <c r="D58" t="n">
         <v>17</v>
       </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Multi-Sport</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -12431,7 +12586,7 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>Steps</t>
+          <t>Schritte</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
@@ -12482,6 +12637,11 @@
           <t>Diving</t>
         </is>
       </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>Tauchen</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -12500,6 +12660,11 @@
       <c r="D61" t="n">
         <v>17</v>
       </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>Sicherheit</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -12518,6 +12683,11 @@
       <c r="D62" t="n">
         <v>17</v>
       </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>Wintersport</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -12942,6 +13112,11 @@
       <c r="D70" t="n">
         <v>29</v>
       </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>Pilates</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -12965,6 +13140,11 @@
           <t>Yoga</t>
         </is>
       </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>Yoga</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -13278,6 +13458,11 @@
           <t>Single-Gas Dive</t>
         </is>
       </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>Einzelgespräche-Tauchgang</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -13301,6 +13486,11 @@
           <t>Multi-Gas Dive</t>
         </is>
       </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>Multigas-Tauchgang</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -13324,6 +13514,11 @@
           <t>Gauge Dive</t>
         </is>
       </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>Tiefenmesser-Tauchgang</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -13347,6 +13542,11 @@
           <t>Apnea</t>
         </is>
       </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>Apnoetauchgang</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -13370,6 +13570,11 @@
           <t>Apnea Hunting</t>
         </is>
       </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>Apnoejagd</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -13388,6 +13593,11 @@
       <c r="D82" t="n">
         <v>144</v>
       </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>CCR-Tauchgang</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -13406,6 +13616,11 @@
       <c r="D83" t="n">
         <v>157</v>
       </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>Hilfe</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -13423,6 +13638,11 @@
       </c>
       <c r="D84" t="n">
         <v>157</v>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>Unfall-Benachrichtigungen</t>
+        </is>
       </c>
     </row>
     <row r="85">

</xml_diff>

<commit_message>
properly updated fields.db with latest
</commit_message>
<xml_diff>
--- a/ConnectStats/sqlite/out/fields.xlsx
+++ b/ConnectStats/sqlite/out/fields.xlsx
@@ -3489,6 +3489,11 @@
           <t>GainCorrectedElevation</t>
         </is>
       </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Elevation Gain</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -3543,6 +3548,11 @@
           <t>GainUncorrectedElevation</t>
         </is>
       </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Elevation Gain</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -3578,6 +3588,11 @@
           <t>LossCorrectedElevation</t>
         </is>
       </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Elevation Loss</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3632,6 +3647,11 @@
           <t>LossUncorrectedElevation</t>
         </is>
       </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Elevation Loss</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3745,6 +3765,11 @@
           <t>MaxCorrectedElevation</t>
         </is>
       </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Max Elevation</t>
+        </is>
+      </c>
       <c r="D31" t="inlineStr">
         <is>
           <t>Max. korrigierte Höhe</t>
@@ -3922,6 +3947,11 @@
           <t>MaxGroundContactTime</t>
         </is>
       </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Max Ground Contact Time</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -3988,6 +4018,11 @@
           <t>MaxMomentaryEnergyExpenditure</t>
         </is>
       </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Max Energy Expenditure</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -4076,6 +4111,11 @@
           <t>MaxRelativeRunningEconomy</t>
         </is>
       </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Max Running Economy</t>
+        </is>
+      </c>
       <c r="D44" t="inlineStr">
         <is>
           <t>Max. relative Laufökonomie</t>
@@ -4241,6 +4281,11 @@
           <t>MaxUncorrectedElevation</t>
         </is>
       </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Max Elevation</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -4248,6 +4293,11 @@
           <t>MaxVerticalOscillation</t>
         </is>
       </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Max Vertical Oscillation</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -4272,6 +4322,11 @@
           <t>MaxVerticalSpeed</t>
         </is>
       </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Max Vertical Speed</t>
+        </is>
+      </c>
       <c r="D52" t="inlineStr">
         <is>
           <t>Max. vertikale Geschw.</t>
@@ -4343,6 +4398,11 @@
           <t>MinBikeCadence</t>
         </is>
       </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Min Cadence</t>
+        </is>
+      </c>
       <c r="D55" t="inlineStr">
         <is>
           <t xml:space="preserve">Min. Trittfrequenz </t>
@@ -4355,6 +4415,11 @@
           <t>MinCorrectedElevation</t>
         </is>
       </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Min Elevation</t>
+        </is>
+      </c>
       <c r="D56" t="inlineStr">
         <is>
           <t>Min. korrigierter Anstieg</t>
@@ -4485,6 +4550,11 @@
           <t>MinGroundContactTime</t>
         </is>
       </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Min Ground Contact Time</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -4521,6 +4591,11 @@
           <t>MinMomentaryEnergyExpenditure</t>
         </is>
       </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Min Energy Expenditure</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -4528,6 +4603,11 @@
           <t>MinPace</t>
         </is>
       </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Min Pace</t>
+        </is>
+      </c>
       <c r="D65" t="inlineStr">
         <is>
           <t>Min. Tempo</t>
@@ -4557,6 +4637,11 @@
           <t>MinRelativeRunningEconomy</t>
         </is>
       </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Min Running Economy</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -4564,6 +4649,11 @@
           <t>MinRunCadence</t>
         </is>
       </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Min Cadence</t>
+        </is>
+      </c>
       <c r="D68" t="inlineStr">
         <is>
           <t>Min. Schrittfrequenz</t>
@@ -4717,6 +4807,11 @@
           <t>MinUncorrectedElevation</t>
         </is>
       </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Min Elevation</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -4724,6 +4819,11 @@
           <t>MinVerticalOscillation</t>
         </is>
       </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Min Vertical Oscillation</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -4743,6 +4843,11 @@
           <t>SumAnaerobicTrainingEffect</t>
         </is>
       </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Anaerobic Training Effect</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -4992,6 +5097,11 @@
           <t>SumFloorsClimbed</t>
         </is>
       </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Floors Climbed</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -4999,6 +5109,11 @@
           <t>SumFloorsDescended</t>
         </is>
       </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Floors Descended</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -5873,6 +5988,11 @@
           <t>WeightedMeanLeftBalance</t>
         </is>
       </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>Avg Left Balance</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -5916,6 +6036,11 @@
           <t>WeightedMeanMomentaryEnergyExpenditure</t>
         </is>
       </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>Avg Energy Expenditure</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -6088,6 +6213,11 @@
           <t>WeightedMeanRelativeRunningEconomy</t>
         </is>
       </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>Avg Running Economy</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -6201,6 +6331,11 @@
           <t>WeightedMeanStanceTime</t>
         </is>
       </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>Avg Stance Time</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -6208,6 +6343,11 @@
           <t>WeightedMeanStanceTimePercent</t>
         </is>
       </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>Avg Stance Percent</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -6484,6 +6624,11 @@
       <c r="A149" t="inlineStr">
         <is>
           <t>WeightedMeanVerticalSpeed</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>Avg Vertical Speed</t>
         </is>
       </c>
     </row>
@@ -8216,11 +8361,6 @@
           <t>SumStrokes</t>
         </is>
       </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>swimming</t>
-        </is>
-      </c>
       <c r="C92" t="inlineStr">
         <is>
           <t>dynamics</t>
@@ -8236,13 +8376,18 @@
           <t>SumStrokes</t>
         </is>
       </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>swimming</t>
+        </is>
+      </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>dynamics</t>
+          <t>swim</t>
         </is>
       </c>
       <c r="D93" t="n">
-        <v>2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="94">

</xml_diff>

<commit_message>
full refactor of calculated series to be thread safe and more logical so the rebuild of best rolling series work better #63"
</commit_message>
<xml_diff>
--- a/ConnectStats/sqlite/out/fields.xlsx
+++ b/ConnectStats/sqlite/out/fields.xlsx
@@ -9017,7 +9017,7 @@
         </is>
       </c>
       <c r="D135" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="136">
@@ -9032,7 +9032,7 @@
         </is>
       </c>
       <c r="D136" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="137">

</xml_diff>